<commit_message>
adding test cases and configuration parts
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,26 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="HomePage" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginPage" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginPageDataProvider" sheetId="3" r:id="rId3"/>
+    <sheet name="RegisterPage" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Demo Web Shop</t>
+  </si>
+  <si>
+    <t>SubMessage</t>
+  </si>
+  <si>
+    <t>Thank you for signing up! A verification email has been sent. We appreciate your interest.</t>
+  </si>
+  <si>
+    <t>Demo Web Shop. Login</t>
+  </si>
+  <si>
+    <t>anuj66@yopmail.com</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
+  <si>
+    <t>anuj@yopmail.com</t>
+  </si>
+  <si>
+    <t>testing@123</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>Login was unsuccessful. Please correct the errors and try again.</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -43,17 +121,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,37 +450,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="26.6328125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>